<commit_message>
Fix issue with draft version
</commit_message>
<xml_diff>
--- a/test-data-generator.xlsx
+++ b/test-data-generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a7bea284aa22fa5/Git Repositories/Intervals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C719F077-F818-40D0-8546-E2F5E8E37587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{C719F077-F818-40D0-8546-E2F5E8E37587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{598E35CF-17EA-4BBE-9E7C-6B8FCB43EA25}"/>
   <bookViews>
     <workbookView xWindow="51195" yWindow="240" windowWidth="25470" windowHeight="20505" xr2:uid="{660962C7-FDB2-437D-9122-6E7748566979}"/>
   </bookViews>
@@ -18,9 +18,6 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$2:$C$126</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$2:$C$63</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$2:$C$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,12 +40,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>mean</t>
   </si>
   <si>
     <t>stdev</t>
+  </si>
+  <si>
+    <t>Interval</t>
   </si>
 </sst>
 </file>
@@ -1098,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CFE529-2D42-4238-AC6B-35C03CA09D0D}">
-  <dimension ref="A1:N132"/>
+  <dimension ref="A1:N135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B126"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,18 +1117,24 @@
         <v>45292</v>
       </c>
       <c r="C1" s="2"/>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f ca="1">EDATE(B1, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46327</v>
+        <f ca="1">EDATE(B1, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46113</v>
       </c>
       <c r="C2" s="2">
         <f ca="1">DATEDIF(B1, B2, "m")</f>
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
         <v>0</v>
@@ -1142,12 +1148,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <f ca="1">EDATE(B2, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47453</v>
+        <f ca="1">EDATE(B2, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46844</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">DATEDIF(B2, B3, "m")</f>
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="M3" t="s">
         <v>1</v>
@@ -1170,12 +1176,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <f ca="1">EDATE(B4, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46447</v>
+        <f ca="1">EDATE(B4, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C4:C21" ca="1" si="0">DATEDIF(B4, B5, "m")</f>
-        <v>38</v>
+        <f t="shared" ref="C5:C21" ca="1" si="0">DATEDIF(B4, B5, "m")</f>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1183,12 +1189,12 @@
         <v>2</v>
       </c>
       <c r="B6" s="1">
-        <f ca="1">EDATE(B5, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47604</v>
+        <f ca="1">EDATE(B5, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46722</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1205,12 +1211,12 @@
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <f ca="1">EDATE(B7, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46266</v>
+        <f ca="1">EDATE(B7, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46054</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1218,12 +1224,12 @@
         <v>3</v>
       </c>
       <c r="B9" s="1">
-        <f ca="1">EDATE(B8, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47300</v>
+        <f ca="1">EDATE(B8, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46784</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1240,12 +1246,12 @@
         <v>4</v>
       </c>
       <c r="B11" s="1">
-        <f ca="1">EDATE(B10, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46357</v>
+        <f ca="1">EDATE(B10, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46023</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1253,12 +1259,12 @@
         <v>4</v>
       </c>
       <c r="B12" s="1">
-        <f ca="1">EDATE(B11, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47423</v>
+        <f ca="1">EDATE(B11, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46722</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1275,12 +1281,12 @@
         <v>5</v>
       </c>
       <c r="B14" s="1">
-        <f ca="1">EDATE(B13, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46419</v>
+        <f ca="1">EDATE(B13, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1288,12 +1294,12 @@
         <v>5</v>
       </c>
       <c r="B15" s="1">
-        <f ca="1">EDATE(B14, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47453</v>
+        <f ca="1">EDATE(B14, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46784</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1310,12 +1316,12 @@
         <v>6</v>
       </c>
       <c r="B17" s="1">
-        <f ca="1">EDATE(B16, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46327</v>
+        <f ca="1">EDATE(B16, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1323,12 +1329,12 @@
         <v>6</v>
       </c>
       <c r="B18" s="1">
-        <f ca="1">EDATE(B17, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47392</v>
+        <f ca="1">EDATE(B17, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46753</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1345,12 +1351,12 @@
         <v>7</v>
       </c>
       <c r="B20" s="1">
-        <f ca="1">EDATE(B19, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46327</v>
+        <f ca="1">EDATE(B19, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1358,12 +1364,12 @@
         <v>7</v>
       </c>
       <c r="B21" s="1">
-        <f ca="1">EDATE(B20, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47362</v>
+        <f ca="1">EDATE(B20, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46692</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1380,12 +1386,12 @@
         <v>8</v>
       </c>
       <c r="B23" s="1">
-        <f ca="1">EDATE(B22, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46296</v>
+        <f ca="1">EDATE(B22, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45962</v>
       </c>
       <c r="C23" s="2">
         <f ca="1">DATEDIF(B22, B23, "m")</f>
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1393,12 +1399,12 @@
         <v>8</v>
       </c>
       <c r="B24" s="1">
-        <f ca="1">EDATE(B23, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47362</v>
+        <f ca="1">EDATE(B23, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46661</v>
       </c>
       <c r="C24" s="2">
         <f ca="1">DATEDIF(B23, B24, "m")</f>
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1415,12 +1421,12 @@
         <v>9</v>
       </c>
       <c r="B26" s="1">
-        <f ca="1">EDATE(B25, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46357</v>
+        <f ca="1">EDATE(B25, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46023</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" ref="C26:C42" ca="1" si="1">DATEDIF(B25, B26, "m")</f>
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1428,12 +1434,12 @@
         <v>9</v>
       </c>
       <c r="B27" s="1">
-        <f ca="1">EDATE(B26, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47543</v>
+        <f ca="1">EDATE(B26, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46722</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1450,12 +1456,12 @@
         <v>10</v>
       </c>
       <c r="B29" s="1">
-        <f ca="1">EDATE(B28, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46388</v>
+        <f ca="1">EDATE(B28, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45931</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1463,12 +1469,12 @@
         <v>10</v>
       </c>
       <c r="B30" s="1">
-        <f ca="1">EDATE(B29, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47515</v>
+        <f ca="1">EDATE(B29, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46692</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1485,12 +1491,12 @@
         <v>11</v>
       </c>
       <c r="B32" s="1">
-        <f ca="1">EDATE(B31, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46447</v>
+        <f ca="1">EDATE(B31, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46023</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1498,12 +1504,12 @@
         <v>11</v>
       </c>
       <c r="B33" s="1">
-        <f ca="1">EDATE(B32, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47453</v>
+        <f ca="1">EDATE(B32, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46753</v>
       </c>
       <c r="C33" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1520,12 +1526,12 @@
         <v>12</v>
       </c>
       <c r="B35" s="1">
-        <f ca="1">EDATE(B34, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46447</v>
+        <f ca="1">EDATE(B34, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45962</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1533,12 +1539,12 @@
         <v>12</v>
       </c>
       <c r="B36" s="1">
-        <f ca="1">EDATE(B35, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47604</v>
+        <f ca="1">EDATE(B35, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46722</v>
       </c>
       <c r="C36" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1555,12 +1561,12 @@
         <v>13</v>
       </c>
       <c r="B38" s="1">
-        <f ca="1">EDATE(B37, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46447</v>
+        <f ca="1">EDATE(B37, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45962</v>
       </c>
       <c r="C38" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,12 +1574,12 @@
         <v>13</v>
       </c>
       <c r="B39" s="1">
-        <f ca="1">EDATE(B38, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47543</v>
+        <f ca="1">EDATE(B38, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46631</v>
       </c>
       <c r="C39" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1590,12 +1596,12 @@
         <v>14</v>
       </c>
       <c r="B41" s="1">
-        <f ca="1">EDATE(B40, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46419</v>
+        <f ca="1">EDATE(B40, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46054</v>
       </c>
       <c r="C41" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1603,12 +1609,12 @@
         <v>14</v>
       </c>
       <c r="B42" s="1">
-        <f ca="1">EDATE(B41, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47453</v>
+        <f ca="1">EDATE(B41, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46784</v>
       </c>
       <c r="C42" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1625,12 +1631,12 @@
         <v>15</v>
       </c>
       <c r="B44" s="1">
-        <f ca="1">EDATE(B43, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46327</v>
+        <f ca="1">EDATE(B43, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C44" s="2">
         <f ca="1">DATEDIF(B43, B44, "m")</f>
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1638,12 +1644,12 @@
         <v>15</v>
       </c>
       <c r="B45" s="1">
-        <f ca="1">EDATE(B44, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47453</v>
+        <f ca="1">EDATE(B44, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46753</v>
       </c>
       <c r="C45" s="2">
         <f ca="1">DATEDIF(B44, B45, "m")</f>
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1660,12 +1666,12 @@
         <v>16</v>
       </c>
       <c r="B47" s="1">
-        <f ca="1">EDATE(B46, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46419</v>
+        <f ca="1">EDATE(B46, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C47" s="2">
         <f t="shared" ref="C47:C63" ca="1" si="2">DATEDIF(B46, B47, "m")</f>
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1673,12 +1679,12 @@
         <v>16</v>
       </c>
       <c r="B48" s="1">
-        <f ca="1">EDATE(B47, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47543</v>
+        <f ca="1">EDATE(B47, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46784</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1695,12 +1701,12 @@
         <v>17</v>
       </c>
       <c r="B50" s="1">
-        <f ca="1">EDATE(B49, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46388</v>
+        <f ca="1">EDATE(B49, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45962</v>
       </c>
       <c r="C50" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1708,12 +1714,12 @@
         <v>17</v>
       </c>
       <c r="B51" s="1">
-        <f ca="1">EDATE(B50, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47574</v>
+        <f ca="1">EDATE(B50, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46661</v>
       </c>
       <c r="C51" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1730,12 +1736,12 @@
         <v>18</v>
       </c>
       <c r="B53" s="1">
-        <f ca="1">EDATE(B52, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46327</v>
+        <f ca="1">EDATE(B52, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46054</v>
       </c>
       <c r="C53" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1743,12 +1749,12 @@
         <v>18</v>
       </c>
       <c r="B54" s="1">
-        <f ca="1">EDATE(B53, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47331</v>
+        <f ca="1">EDATE(B53, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46722</v>
       </c>
       <c r="C54" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1765,12 +1771,12 @@
         <v>19</v>
       </c>
       <c r="B56" s="1">
-        <f ca="1">EDATE(B55, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46478</v>
+        <f ca="1">EDATE(B55, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45931</v>
       </c>
       <c r="C56" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1778,12 +1784,12 @@
         <v>19</v>
       </c>
       <c r="B57" s="1">
-        <f ca="1">EDATE(B56, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47635</v>
+        <f ca="1">EDATE(B56, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46569</v>
       </c>
       <c r="C57" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1800,12 +1806,12 @@
         <v>20</v>
       </c>
       <c r="B59" s="1">
-        <f ca="1">EDATE(B58, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46357</v>
+        <f ca="1">EDATE(B58, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45962</v>
       </c>
       <c r="C59" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1813,12 +1819,12 @@
         <v>20</v>
       </c>
       <c r="B60" s="1">
-        <f ca="1">EDATE(B59, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47453</v>
+        <f ca="1">EDATE(B59, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46661</v>
       </c>
       <c r="C60" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1835,12 +1841,12 @@
         <v>21</v>
       </c>
       <c r="B62" s="1">
-        <f ca="1">EDATE(B61, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46478</v>
+        <f ca="1">EDATE(B61, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46023</v>
       </c>
       <c r="C62" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1848,12 +1854,12 @@
         <v>21</v>
       </c>
       <c r="B63" s="1">
-        <f ca="1">EDATE(B62, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47453</v>
+        <f ca="1">EDATE(B62, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46722</v>
       </c>
       <c r="C63" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1870,12 +1876,12 @@
         <v>22</v>
       </c>
       <c r="B65" s="1">
-        <f ca="1">EDATE(B64, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46327</v>
+        <f ca="1">EDATE(B64, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C65" s="2">
         <f ca="1">DATEDIF(B64, B65, "m")</f>
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1883,12 +1889,12 @@
         <v>22</v>
       </c>
       <c r="B66" s="1">
-        <f ca="1">EDATE(B65, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47515</v>
+        <f ca="1">EDATE(B65, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46600</v>
       </c>
       <c r="C66" s="2">
         <f ca="1">DATEDIF(B65, B66, "m")</f>
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1905,12 +1911,12 @@
         <v>23</v>
       </c>
       <c r="B68" s="1">
-        <f ca="1">EDATE(B67, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46388</v>
+        <f ca="1">EDATE(B67, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45962</v>
       </c>
       <c r="C68" s="2">
         <f t="shared" ref="C68:C84" ca="1" si="3">DATEDIF(B67, B68, "m")</f>
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1918,12 +1924,12 @@
         <v>23</v>
       </c>
       <c r="B69" s="1">
-        <f ca="1">EDATE(B68, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47362</v>
+        <f ca="1">EDATE(B68, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46692</v>
       </c>
       <c r="C69" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1940,12 +1946,12 @@
         <v>24</v>
       </c>
       <c r="B71" s="1">
-        <f ca="1">EDATE(B70, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46419</v>
+        <f ca="1">EDATE(B70, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C71" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1953,12 +1959,12 @@
         <v>24</v>
       </c>
       <c r="B72" s="1">
-        <f ca="1">EDATE(B71, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47423</v>
+        <f ca="1">EDATE(B71, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46722</v>
       </c>
       <c r="C72" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1975,12 +1981,12 @@
         <v>25</v>
       </c>
       <c r="B74" s="1">
-        <f ca="1">EDATE(B73, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46388</v>
+        <f ca="1">EDATE(B73, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46023</v>
       </c>
       <c r="C74" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1988,12 +1994,12 @@
         <v>25</v>
       </c>
       <c r="B75" s="1">
-        <f ca="1">EDATE(B74, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47484</v>
+        <f ca="1">EDATE(B74, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46722</v>
       </c>
       <c r="C75" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2010,12 +2016,12 @@
         <v>26</v>
       </c>
       <c r="B77" s="1">
-        <f ca="1">EDATE(B76, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46447</v>
+        <f ca="1">EDATE(B76, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C77" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2023,12 +2029,12 @@
         <v>26</v>
       </c>
       <c r="B78" s="1">
-        <f ca="1">EDATE(B77, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47543</v>
+        <f ca="1">EDATE(B77, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46692</v>
       </c>
       <c r="C78" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2045,12 +2051,12 @@
         <v>27</v>
       </c>
       <c r="B80" s="1">
-        <f ca="1">EDATE(B79, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46419</v>
+        <f ca="1">EDATE(B79, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46023</v>
       </c>
       <c r="C80" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2058,12 +2064,12 @@
         <v>27</v>
       </c>
       <c r="B81" s="1">
-        <f ca="1">EDATE(B80, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47515</v>
+        <f ca="1">EDATE(B80, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46784</v>
       </c>
       <c r="C81" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2080,12 +2086,12 @@
         <v>28</v>
       </c>
       <c r="B83" s="1">
-        <f ca="1">EDATE(B82, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46419</v>
+        <f ca="1">EDATE(B82, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46054</v>
       </c>
       <c r="C83" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2093,12 +2099,12 @@
         <v>28</v>
       </c>
       <c r="B84" s="1">
-        <f ca="1">EDATE(B83, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47515</v>
+        <f ca="1">EDATE(B83, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46753</v>
       </c>
       <c r="C84" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2115,12 +2121,12 @@
         <v>29</v>
       </c>
       <c r="B86" s="1">
-        <f ca="1">EDATE(B85, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46419</v>
+        <f ca="1">EDATE(B85, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45901</v>
       </c>
       <c r="C86" s="2">
         <f ca="1">DATEDIF(B85, B86, "m")</f>
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2128,12 +2134,12 @@
         <v>29</v>
       </c>
       <c r="B87" s="1">
-        <f ca="1">EDATE(B86, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47453</v>
+        <f ca="1">EDATE(B86, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46539</v>
       </c>
       <c r="C87" s="2">
         <f ca="1">DATEDIF(B86, B87, "m")</f>
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2150,12 +2156,12 @@
         <v>30</v>
       </c>
       <c r="B89" s="1">
-        <f ca="1">EDATE(B88, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46327</v>
+        <f ca="1">EDATE(B88, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45962</v>
       </c>
       <c r="C89" s="2">
         <f t="shared" ref="C89:C105" ca="1" si="4">DATEDIF(B88, B89, "m")</f>
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2163,12 +2169,12 @@
         <v>30</v>
       </c>
       <c r="B90" s="1">
-        <f ca="1">EDATE(B89, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47392</v>
+        <f ca="1">EDATE(B89, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46600</v>
       </c>
       <c r="C90" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2185,12 +2191,12 @@
         <v>31</v>
       </c>
       <c r="B92" s="1">
-        <f ca="1">EDATE(B91, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46296</v>
+        <f ca="1">EDATE(B91, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46082</v>
       </c>
       <c r="C92" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2198,12 +2204,12 @@
         <v>31</v>
       </c>
       <c r="B93" s="1">
-        <f ca="1">EDATE(B92, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47239</v>
+        <f ca="1">EDATE(B92, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46784</v>
       </c>
       <c r="C93" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2220,12 +2226,12 @@
         <v>32</v>
       </c>
       <c r="B95" s="1">
-        <f ca="1">EDATE(B94, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46388</v>
+        <f ca="1">EDATE(B94, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46113</v>
       </c>
       <c r="C95" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2233,12 +2239,12 @@
         <v>32</v>
       </c>
       <c r="B96" s="1">
-        <f ca="1">EDATE(B95, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47362</v>
+        <f ca="1">EDATE(B95, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46784</v>
       </c>
       <c r="C96" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2255,12 +2261,12 @@
         <v>33</v>
       </c>
       <c r="B98" s="1">
-        <f ca="1">EDATE(B97, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46388</v>
+        <f ca="1">EDATE(B97, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C98" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,12 +2274,12 @@
         <v>33</v>
       </c>
       <c r="B99" s="1">
-        <f ca="1">EDATE(B98, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47484</v>
+        <f ca="1">EDATE(B98, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46692</v>
       </c>
       <c r="C99" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,12 +2296,12 @@
         <v>34</v>
       </c>
       <c r="B101" s="1">
-        <f ca="1">EDATE(B100, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46357</v>
+        <f ca="1">EDATE(B100, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46054</v>
       </c>
       <c r="C101" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2303,12 +2309,12 @@
         <v>34</v>
       </c>
       <c r="B102" s="1">
-        <f ca="1">EDATE(B101, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47484</v>
+        <f ca="1">EDATE(B101, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46784</v>
       </c>
       <c r="C102" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2325,12 +2331,12 @@
         <v>35</v>
       </c>
       <c r="B104" s="1">
-        <f ca="1">EDATE(B103, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46447</v>
+        <f ca="1">EDATE(B103, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45962</v>
       </c>
       <c r="C104" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2338,12 +2344,12 @@
         <v>35</v>
       </c>
       <c r="B105" s="1">
-        <f ca="1">EDATE(B104, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47543</v>
+        <f ca="1">EDATE(B104, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46753</v>
       </c>
       <c r="C105" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2360,12 +2366,12 @@
         <v>36</v>
       </c>
       <c r="B107" s="1">
-        <f ca="1">EDATE(B106, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46357</v>
+        <f ca="1">EDATE(B106, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46023</v>
       </c>
       <c r="C107" s="2">
         <f ca="1">DATEDIF(B106, B107, "m")</f>
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2373,12 +2379,12 @@
         <v>36</v>
       </c>
       <c r="B108" s="1">
-        <f ca="1">EDATE(B107, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47423</v>
+        <f ca="1">EDATE(B107, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46661</v>
       </c>
       <c r="C108" s="2">
         <f ca="1">DATEDIF(B107, B108, "m")</f>
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -2395,12 +2401,12 @@
         <v>37</v>
       </c>
       <c r="B110" s="1">
-        <f ca="1">EDATE(B109, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46296</v>
+        <f ca="1">EDATE(B109, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46082</v>
       </c>
       <c r="C110" s="2">
         <f t="shared" ref="C110:C126" ca="1" si="5">DATEDIF(B109, B110, "m")</f>
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2408,12 +2414,12 @@
         <v>37</v>
       </c>
       <c r="B111" s="1">
-        <f ca="1">EDATE(B110, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47362</v>
+        <f ca="1">EDATE(B110, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46753</v>
       </c>
       <c r="C111" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2430,12 +2436,12 @@
         <v>38</v>
       </c>
       <c r="B113" s="1">
-        <f ca="1">EDATE(B112, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46357</v>
+        <f ca="1">EDATE(B112, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46082</v>
       </c>
       <c r="C113" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2443,12 +2449,12 @@
         <v>38</v>
       </c>
       <c r="B114" s="1">
-        <f ca="1">EDATE(B113, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47362</v>
+        <f ca="1">EDATE(B113, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46844</v>
       </c>
       <c r="C114" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2465,12 +2471,12 @@
         <v>39</v>
       </c>
       <c r="B116" s="1">
-        <f ca="1">EDATE(B115, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46357</v>
+        <f ca="1">EDATE(B115, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45901</v>
       </c>
       <c r="C116" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -2478,12 +2484,12 @@
         <v>39</v>
       </c>
       <c r="B117" s="1">
-        <f ca="1">EDATE(B116, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47515</v>
+        <f ca="1">EDATE(B116, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46600</v>
       </c>
       <c r="C117" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -2500,12 +2506,12 @@
         <v>40</v>
       </c>
       <c r="B119" s="1">
-        <f ca="1">EDATE(B118, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46357</v>
+        <f ca="1">EDATE(B118, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45992</v>
       </c>
       <c r="C119" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -2513,12 +2519,12 @@
         <v>40</v>
       </c>
       <c r="B120" s="1">
-        <f ca="1">EDATE(B119, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47574</v>
+        <f ca="1">EDATE(B119, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46722</v>
       </c>
       <c r="C120" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -2535,12 +2541,12 @@
         <v>41</v>
       </c>
       <c r="B122" s="1">
-        <f ca="1">EDATE(B121, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46357</v>
+        <f ca="1">EDATE(B121, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46082</v>
       </c>
       <c r="C122" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -2548,12 +2554,12 @@
         <v>41</v>
       </c>
       <c r="B123" s="1">
-        <f ca="1">EDATE(B122, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47453</v>
+        <f ca="1">EDATE(B122, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46844</v>
       </c>
       <c r="C123" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -2570,12 +2576,12 @@
         <v>42</v>
       </c>
       <c r="B125" s="1">
-        <f ca="1">EDATE(B124, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>46266</v>
+        <f ca="1">EDATE(B124, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>45931</v>
       </c>
       <c r="C125" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -2583,12 +2589,12 @@
         <v>42</v>
       </c>
       <c r="B126" s="1">
-        <f ca="1">EDATE(B125, 36 + NORMINV(RAND(),$N$2,$N$3))</f>
-        <v>47331</v>
+        <f ca="1">EDATE(B125, $N$1 + NORMINV(RAND(),$N$2,$N$3))</f>
+        <v>46631</v>
       </c>
       <c r="C126" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -2608,6 +2614,15 @@
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>